<commit_message>
removed emissions factors from git since to large and merging issues
</commit_message>
<xml_diff>
--- a/config/reference_table_sector.xlsx
+++ b/config/reference_table_sector.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC3F10C-2A73-40D5-B1E3-60D0E3E62D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6429BA12-0E48-4201-92C6-BDA6246A5EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C2CF52B6-4E3D-4DA0-8DC0-D6A8EB942BC2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2CF52B6-4E3D-4DA0-8DC0-D6A8EB942BC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="sectors" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1495,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4F16BD-6EAF-4DFC-894F-17C14E0AC30D}">
   <dimension ref="A1:F293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
@@ -4547,6 +4547,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3042e625-934f-4bb2-8533-cbb6446c8b2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033DE4B8CEBD9304286F1E0B7BC383844" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d76399d66d45378b52bd24e5db7672eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa" xmlns:ns3="3042e625-934f-4bb2-8533-cbb6446c8b2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f81e3bb06f6900da50fdd409f0138bcf" ns2:_="" ns3:_="">
     <xsd:import namespace="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
@@ -4757,17 +4768,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3042e625-934f-4bb2-8533-cbb6446c8b2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA31DF46-11A9-4EBF-939B-7AC177202FC8}">
   <ds:schemaRefs>
@@ -4777,6 +4777,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99D167C1-C23B-4884-BFCC-8FA899DFAD4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
+    <ds:schemaRef ds:uri="3042e625-934f-4bb2-8533-cbb6446c8b2b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF95C38B-BFCD-4DB4-B445-2AEE8E534FF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4793,15 +4804,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99D167C1-C23B-4884-BFCC-8FA899DFAD4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
-    <ds:schemaRef ds:uri="3042e625-934f-4bb2-8533-cbb6446c8b2b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new esto file name
</commit_message>
<xml_diff>
--- a/config/reference_table_sector.xlsx
+++ b/config/reference_table_sector.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\Outlook9th_EBT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC3F10C-2A73-40D5-B1E3-60D0E3E62D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6429BA12-0E48-4201-92C6-BDA6246A5EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C2CF52B6-4E3D-4DA0-8DC0-D6A8EB942BC2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2CF52B6-4E3D-4DA0-8DC0-D6A8EB942BC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="sectors" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1495,7 +1495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4F16BD-6EAF-4DFC-894F-17C14E0AC30D}">
   <dimension ref="A1:F293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
@@ -4547,6 +4547,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3042e625-934f-4bb2-8533-cbb6446c8b2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033DE4B8CEBD9304286F1E0B7BC383844" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d76399d66d45378b52bd24e5db7672eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa" xmlns:ns3="3042e625-934f-4bb2-8533-cbb6446c8b2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f81e3bb06f6900da50fdd409f0138bcf" ns2:_="" ns3:_="">
     <xsd:import namespace="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
@@ -4757,17 +4768,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3042e625-934f-4bb2-8533-cbb6446c8b2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA31DF46-11A9-4EBF-939B-7AC177202FC8}">
   <ds:schemaRefs>
@@ -4777,6 +4777,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99D167C1-C23B-4884-BFCC-8FA899DFAD4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
+    <ds:schemaRef ds:uri="3042e625-934f-4bb2-8533-cbb6446c8b2b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF95C38B-BFCD-4DB4-B445-2AEE8E534FF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4793,15 +4804,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99D167C1-C23B-4884-BFCC-8FA899DFAD4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
-    <ds:schemaRef ds:uri="3042e625-934f-4bb2-8533-cbb6446c8b2b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>